<commit_message>
Created database structure. Added option in game to refresh database Started working on modifying gameplay to use database.    Got to unit selector in gameplay    Still need to add in mechanics to select sentences from the database to play.
</commit_message>
<xml_diff>
--- a/data/OpinSuomea - Lause tiedot.xlsx
+++ b/data/OpinSuomea - Lause tiedot.xlsx
@@ -6,7 +6,8 @@
     <sheet state="visible" name="Usage" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Verbit" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Template" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Unit 1 - test" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Unit 0 - test unit" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Unit 1 - add more here!" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="318">
   <si>
     <t>This spreadsheet is intended to hold sample sentences for the OpinSuomea python program</t>
   </si>
   <si>
-    <t>Verbit: A list of verbs and their translations.  These are referred to by the program to translate sentences</t>
+    <t>Verbit: A list of verbs and their translations.  These are referred to by the program to share English translations of the sentences</t>
   </si>
   <si>
     <t>Template: This is an example of how "units" should be constructed.</t>
@@ -34,7 +35,7 @@
     <t>Please do not use ### anywhere in sentences other than to replace missing verbs (or nouns, if we get there)</t>
   </si>
   <si>
-    <t>For kirjakieli tai puhekieli - let's focus on kirjakieli initially, but this is here in case we want to change at some point</t>
+    <t>kirjakieli tai puhekieli - let's focus on kirjakieli initially, but this is here in case we want to change at some point (or allow us to select to practice one or the other)</t>
   </si>
   <si>
     <t>Infinitive</t>
@@ -454,7 +455,7 @@
     <t>To rise / arise</t>
   </si>
   <si>
-    <t>Nousta ylös</t>
+    <t>nousta ylös</t>
   </si>
   <si>
     <t>To get up</t>
@@ -526,12 +527,6 @@
     <t>to take, to remove</t>
   </si>
   <si>
-    <t>Paljonko se maksaa?</t>
-  </si>
-  <si>
-    <t>How much does it cost?</t>
-  </si>
-  <si>
     <t>pelata</t>
   </si>
   <si>
@@ -814,7 +809,7 @@
     <t>Unit number</t>
   </si>
   <si>
-    <t>Number (integer, positive) of the unit</t>
+    <t>Number of the unit (can include text, if you want)</t>
   </si>
   <si>
     <t>Unit name</t>
@@ -832,7 +827,7 @@
     <t>Update date</t>
   </si>
   <si>
-    <t>2022.01.27</t>
+    <t>2022.01.29</t>
   </si>
   <si>
     <t>Other info</t>
@@ -841,6 +836,9 @@
     <t>Created by, notes, etc.</t>
   </si>
   <si>
+    <t>ID (unique)</t>
+  </si>
+  <si>
     <t>Puhekieli tai kirjakieli</t>
   </si>
   <si>
@@ -856,6 +854,9 @@
     <t>English translation of sentence</t>
   </si>
   <si>
+    <t>UX-1</t>
+  </si>
+  <si>
     <t>kirjakieli</t>
   </si>
   <si>
@@ -868,7 +869,19 @@
     <t>I love this!</t>
   </si>
   <si>
-    <t>Test unit</t>
+    <t>UX-2</t>
+  </si>
+  <si>
+    <t>Minun ei tarvitse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[minä] ### lukea tenttin </t>
+  </si>
+  <si>
+    <t>I do not need to study for the test</t>
+  </si>
+  <si>
+    <t>Test unit - here for QA work, really.  Use other units for real practice.</t>
   </si>
   <si>
     <t>A unit to test functioning of the program</t>
@@ -877,6 +890,9 @@
     <t xml:space="preserve">by MP. </t>
   </si>
   <si>
+    <t>U0-1</t>
+  </si>
+  <si>
     <t>asun</t>
   </si>
   <si>
@@ -886,6 +902,9 @@
     <t>I live in Finland</t>
   </si>
   <si>
+    <t>U0-2</t>
+  </si>
+  <si>
     <t>asuu</t>
   </si>
   <si>
@@ -895,6 +914,9 @@
     <t>She lives in Finland</t>
   </si>
   <si>
+    <t>U0-3</t>
+  </si>
+  <si>
     <t>menet</t>
   </si>
   <si>
@@ -904,6 +926,9 @@
     <t>You are going to campus.</t>
   </si>
   <si>
+    <t>U0-4</t>
+  </si>
+  <si>
     <t>kävimme</t>
   </si>
   <si>
@@ -913,13 +938,37 @@
     <t>We went to the movies.</t>
   </si>
   <si>
-    <t>Minun ei tarvitse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[minä] ### lukea tenttin </t>
-  </si>
-  <si>
-    <t>I do not need to study for the test</t>
+    <t>U0-5</t>
+  </si>
+  <si>
+    <t>U0-6</t>
+  </si>
+  <si>
+    <t>puhekieli</t>
+  </si>
+  <si>
+    <t>oon</t>
+  </si>
+  <si>
+    <t>Mä ### onnellinen</t>
+  </si>
+  <si>
+    <t>I am happy.</t>
+  </si>
+  <si>
+    <t>First real unit</t>
+  </si>
+  <si>
+    <t>Simple sentences</t>
+  </si>
+  <si>
+    <t>U1-1</t>
+  </si>
+  <si>
+    <t>U1-2</t>
+  </si>
+  <si>
+    <t>U1-3</t>
   </si>
 </sst>
 </file>
@@ -979,6 +1028,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2113,15 +2166,15 @@
         <v>224</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="112">
@@ -2266,14 +2319,6 @@
       </c>
       <c r="B129" s="1" t="s">
         <v>262</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2291,97 +2336,123 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.71"/>
-    <col customWidth="1" min="3" max="3" width="24.29"/>
-    <col customWidth="1" min="4" max="4" width="42.0"/>
-    <col customWidth="1" min="5" max="5" width="46.43"/>
+    <col customWidth="1" min="1" max="2" width="17.71"/>
+    <col customWidth="1" min="4" max="4" width="24.29"/>
+    <col customWidth="1" min="5" max="5" width="42.0"/>
+    <col customWidth="1" min="6" max="6" width="46.43"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="C8" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2398,15 +2469,216 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.86"/>
-    <col customWidth="1" min="3" max="3" width="24.29"/>
-    <col customWidth="1" min="4" max="4" width="42.0"/>
-    <col customWidth="1" min="5" max="5" width="46.43"/>
+    <col customWidth="1" min="1" max="2" width="16.29"/>
+    <col customWidth="1" min="4" max="4" width="24.29"/>
+    <col customWidth="1" min="5" max="5" width="42.0"/>
+    <col customWidth="1" min="6" max="6" width="46.43"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>265</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="2" width="16.29"/>
+    <col customWidth="1" min="4" max="4" width="24.29"/>
+    <col customWidth="1" min="5" max="5" width="42.0"/>
+    <col customWidth="1" min="6" max="6" width="46.43"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="B1" s="1">
         <v>1.0</v>
@@ -2414,136 +2686,114 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>284</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>285</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>287</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>290</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>292</v>
+        <v>297</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E12" s="1" t="s">
         <v>301</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code to store results of each game round in both the in-memory sentence list and in the database.  Database is now completely functional at a base level - import from spreadsheet, pull from DB to form in-memory sentence lists, and push results to DB for storage.  Yippee! Also added ability to have non-verb sentences, and have them include hints.  Included dummy "-" value for verb table and verb-infinitive in non-verb table, so that SQL would be easier. Import template also changed, of course, to allow for non-verb sentences.
</commit_message>
<xml_diff>
--- a/data/OpinSuomea - Lause tiedot.xlsx
+++ b/data/OpinSuomea - Lause tiedot.xlsx
@@ -15,18 +15,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="342">
   <si>
     <t>This spreadsheet is intended to hold sample sentences for the OpinSuomea python program</t>
   </si>
   <si>
+    <t>Design idea:  A program that presents setnences with one gap in them, along with hints, and then prompts the user to type the correct word(s) to fill the gap</t>
+  </si>
+  <si>
+    <t>Key: Only one word or phrase, in one part of the sentence, can be missing</t>
+  </si>
+  <si>
+    <t>These words can be verbs, nouns (not implemented yet), or other phrases - but only one of those three.</t>
+  </si>
+  <si>
     <t>Verbit: A list of verbs and their translations.  These are referred to by the program to share English translations of the sentences</t>
   </si>
   <si>
+    <t>If you use a verb not in this list in a unit, you must add it to the list!</t>
+  </si>
+  <si>
+    <t>When verbs are missing, the program will show the verb infinitive and its translation (pulling the translation from this table)</t>
+  </si>
+  <si>
     <t>Template: This is an example of how "units" should be constructed.</t>
   </si>
   <si>
-    <t>Each unit consists of a set of sentences along with a correctly conjugated verb.</t>
+    <t>Each unit consists of a set of sentences with a single gap missing, along with the correct answer for the gap.</t>
+  </si>
+  <si>
+    <t>Units have either a verb or another phrase missing - not both.</t>
   </si>
   <si>
     <t>Units can have as many or as few sentences as you want</t>
@@ -35,7 +53,7 @@
     <t>Please do not use ### anywhere in sentences other than to replace missing verbs (or nouns, if we get there)</t>
   </si>
   <si>
-    <t>kirjakieli tai puhekieli - let's focus on kirjakieli initially, but this is here in case we want to change at some point (or allow us to select to practice one or the other)</t>
+    <t>kirjakieli tai puhekieli - brings up a warning when sentences are in puhekieli, and also lets users select one or the other (not implemented yet)</t>
   </si>
   <si>
     <t>Infinitive</t>
@@ -842,13 +860,19 @@
     <t>Puhekieli tai kirjakieli</t>
   </si>
   <si>
+    <t>Type of thing missing</t>
+  </si>
+  <si>
     <t>Verb (infinitive)</t>
   </si>
   <si>
-    <t>Verb correctly conjugated</t>
-  </si>
-  <si>
-    <t>Lause (replace verb with ###)</t>
+    <t>If not a verb, translation or hint here (optional)</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Lause (replace verb or phrase with ###)</t>
   </si>
   <si>
     <t>English translation of sentence</t>
@@ -860,6 +884,9 @@
     <t>kirjakieli</t>
   </si>
   <si>
+    <t>verb</t>
+  </si>
+  <si>
     <t>rakastan</t>
   </si>
   <si>
@@ -881,6 +908,54 @@
     <t>I do not need to study for the test</t>
   </si>
   <si>
+    <t>UX-3</t>
+  </si>
+  <si>
+    <t>puhekieli</t>
+  </si>
+  <si>
+    <t>oon</t>
+  </si>
+  <si>
+    <t>Mä ### iloinen</t>
+  </si>
+  <si>
+    <t>I am happy.</t>
+  </si>
+  <si>
+    <t>UX-4</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>sohva_ a___</t>
+  </si>
+  <si>
+    <t>sohvan alla</t>
+  </si>
+  <si>
+    <t>Kissä on ###</t>
+  </si>
+  <si>
+    <t>The cat is under the couch</t>
+  </si>
+  <si>
+    <t>UX-5</t>
+  </si>
+  <si>
+    <t>kaapi_ pää___</t>
+  </si>
+  <si>
+    <t>kaapin päällä</t>
+  </si>
+  <si>
+    <t>Avain oli ###</t>
+  </si>
+  <si>
+    <t>The key was on top of the cabinet</t>
+  </si>
+  <si>
     <t>Test unit - here for QA work, really.  Use other units for real practice.</t>
   </si>
   <si>
@@ -944,16 +1019,13 @@
     <t>U0-6</t>
   </si>
   <si>
-    <t>puhekieli</t>
-  </si>
-  <si>
-    <t>oon</t>
-  </si>
-  <si>
     <t>Mä ### onnellinen</t>
   </si>
   <si>
-    <t>I am happy.</t>
+    <t>U0-7</t>
+  </si>
+  <si>
+    <t>U0-8</t>
   </si>
   <si>
     <t>First real unit</t>
@@ -1249,18 +1321,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7">
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1272,6 +1349,36 @@
     <row r="9">
       <c r="B9" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1291,1034 +1398,1034 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2336,123 +2443,195 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="17.71"/>
-    <col customWidth="1" min="4" max="4" width="24.29"/>
-    <col customWidth="1" min="5" max="5" width="42.0"/>
-    <col customWidth="1" min="6" max="6" width="46.43"/>
+    <col customWidth="1" min="1" max="1" width="13.86"/>
+    <col customWidth="1" min="2" max="2" width="14.0"/>
+    <col customWidth="1" min="5" max="6" width="24.29"/>
+    <col customWidth="1" min="7" max="7" width="42.0"/>
+    <col customWidth="1" min="8" max="8" width="46.43"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>278</v>
+        <v>284</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>190</v>
+        <v>289</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>282</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>283</v>
+        <v>290</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>224</v>
+        <v>289</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>286</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>287</v>
+        <v>294</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>312</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2470,14 +2649,15 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="2" width="16.29"/>
-    <col customWidth="1" min="4" max="4" width="24.29"/>
-    <col customWidth="1" min="5" max="5" width="42.0"/>
-    <col customWidth="1" min="6" max="6" width="46.43"/>
+    <col customWidth="1" min="5" max="5" width="17.29"/>
+    <col customWidth="1" min="6" max="6" width="24.29"/>
+    <col customWidth="1" min="7" max="7" width="42.0"/>
+    <col customWidth="1" min="8" max="8" width="46.43"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="B1" s="1">
         <v>0.0</v>
@@ -2485,173 +2665,249 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>288</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>278</v>
+        <v>284</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>289</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>293</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>294</v>
+        <v>317</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>295</v>
+        <v>320</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>289</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>297</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>298</v>
+        <v>321</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>299</v>
+        <v>324</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>126</v>
+        <v>289</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>301</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>302</v>
+        <v>325</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>303</v>
+        <v>328</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>289</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>305</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>306</v>
+        <v>329</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>307</v>
+        <v>332</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>224</v>
+        <v>289</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>286</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>287</v>
+        <v>294</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>308</v>
+        <v>333</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>312</v>
       </c>
     </row>
@@ -2670,15 +2926,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="16.29"/>
-    <col customWidth="1" min="4" max="4" width="24.29"/>
-    <col customWidth="1" min="5" max="5" width="42.0"/>
-    <col customWidth="1" min="6" max="6" width="46.43"/>
+    <col customWidth="1" min="1" max="1" width="12.43"/>
+    <col customWidth="1" min="2" max="2" width="16.0"/>
+    <col customWidth="1" min="5" max="5" width="18.29"/>
+    <col customWidth="1" min="6" max="6" width="10.86"/>
+    <col customWidth="1" min="7" max="7" width="42.0"/>
+    <col customWidth="1" min="8" max="8" width="46.43"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="B1" s="1">
         <v>1.0</v>
@@ -2686,114 +2944,132 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>313</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>278</v>
+        <v>284</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>315</v>
+        <v>339</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>289</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>293</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>294</v>
+        <v>317</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>316</v>
+        <v>340</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>289</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>297</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>298</v>
+        <v>321</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>317</v>
+        <v>341</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>126</v>
+        <v>289</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>301</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>302</v>
+        <v>325</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created algorithm to bias probability of selecting sentences based on sentence score and whether the sentence has been played.  Separately, have code to prevent re-playing of already-played-this-round sentences. Added code to store each round's result in the history database table.
</commit_message>
<xml_diff>
--- a/data/OpinSuomea - Lause tiedot.xlsx
+++ b/data/OpinSuomea - Lause tiedot.xlsx
@@ -8,6 +8,7 @@
     <sheet state="visible" name="Template" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Unit 0 - test unit" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Unit 1 - add more here!" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Unit 2 - sentences of necessity" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="485">
   <si>
     <t>This spreadsheet is intended to hold sample sentences for the OpinSuomea python program</t>
   </si>
@@ -824,9 +825,6 @@
     <t>To try</t>
   </si>
   <si>
-    <t>Unit number</t>
-  </si>
-  <si>
     <t>Number of the unit (can include text, if you want)</t>
   </si>
   <si>
@@ -956,7 +954,7 @@
     <t>The key was on top of the cabinet</t>
   </si>
   <si>
-    <t>Test unit - here for QA work, really.  Use other units for real practice.</t>
+    <t xml:space="preserve">Test unit for QA purposes. </t>
   </si>
   <si>
     <t>A unit to test functioning of the program</t>
@@ -1041,6 +1039,438 @@
   </si>
   <si>
     <t>U1-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sentences of necessisity </t>
+  </si>
+  <si>
+    <t>Always requires the pronoun.</t>
+  </si>
+  <si>
+    <t>2022.01.30</t>
+  </si>
+  <si>
+    <t>U2-1</t>
+  </si>
+  <si>
+    <t>I - include the proper pronoun!</t>
+  </si>
+  <si>
+    <t>Minä haluan</t>
+  </si>
+  <si>
+    <t>### perunoita!</t>
+  </si>
+  <si>
+    <t>I want potatoes!</t>
+  </si>
+  <si>
+    <t>U2-2</t>
+  </si>
+  <si>
+    <t>Minä tarvitsen</t>
+  </si>
+  <si>
+    <t>I need potatoes!</t>
+  </si>
+  <si>
+    <t>U2-3</t>
+  </si>
+  <si>
+    <t>You (singular) - include the proper pronoun</t>
+  </si>
+  <si>
+    <t>Sinä tarvitset</t>
+  </si>
+  <si>
+    <t>You (singular) need potatoes</t>
+  </si>
+  <si>
+    <t>U2-4</t>
+  </si>
+  <si>
+    <t>Michelle - include pronoun</t>
+  </si>
+  <si>
+    <t>Michellen täytyy</t>
+  </si>
+  <si>
+    <t>### saada perunat.</t>
+  </si>
+  <si>
+    <t>Michelle needs to get potatoes</t>
+  </si>
+  <si>
+    <t>U2-5</t>
+  </si>
+  <si>
+    <t>Kissa - include pronoun</t>
+  </si>
+  <si>
+    <t>Kissan ei tarvitse</t>
+  </si>
+  <si>
+    <t>### syödä perunaa.</t>
+  </si>
+  <si>
+    <t>The cat does not need to eat a potato.</t>
+  </si>
+  <si>
+    <t>U2-6</t>
+  </si>
+  <si>
+    <t>We - include the pronoun</t>
+  </si>
+  <si>
+    <t>Meidän pitää</t>
+  </si>
+  <si>
+    <t>### kokata perunoita</t>
+  </si>
+  <si>
+    <t>We need to cook potatoes</t>
+  </si>
+  <si>
+    <t>U2-7</t>
+  </si>
+  <si>
+    <t>Kaupa - include pronoun.  Note the "should"!</t>
+  </si>
+  <si>
+    <t>Kaupan pitäisi</t>
+  </si>
+  <si>
+    <t>### myydä perunoita</t>
+  </si>
+  <si>
+    <t>The store should sell potatoes</t>
+  </si>
+  <si>
+    <t>U2-8</t>
+  </si>
+  <si>
+    <t>You (plural) - include pronoun</t>
+  </si>
+  <si>
+    <t>Teidän ei pitäisi</t>
+  </si>
+  <si>
+    <t>### unohtaa perunoita</t>
+  </si>
+  <si>
+    <t>You (plural) should not forget potatoes</t>
+  </si>
+  <si>
+    <t>U2-9</t>
+  </si>
+  <si>
+    <t>They - include pronoun (and maybe you need another word too?)</t>
+  </si>
+  <si>
+    <t>Heidän on pakko</t>
+  </si>
+  <si>
+    <t>### ostaa perunoita</t>
+  </si>
+  <si>
+    <t>They must buy potaotes (it is the law!)</t>
+  </si>
+  <si>
+    <t>U2-10</t>
+  </si>
+  <si>
+    <t>We - include pronoun (and maybe another word?)</t>
+  </si>
+  <si>
+    <t>Meidän olisi hyvä</t>
+  </si>
+  <si>
+    <t>### pyöräillä järvin ympäri</t>
+  </si>
+  <si>
+    <t>It would be a good idea for us to ride our bikes around the lake.</t>
+  </si>
+  <si>
+    <t>U2-11</t>
+  </si>
+  <si>
+    <t>Meidän on pakko</t>
+  </si>
+  <si>
+    <t>### pyöräillä pyöriäme</t>
+  </si>
+  <si>
+    <t>We must ride bicycles</t>
+  </si>
+  <si>
+    <t>U2-12</t>
+  </si>
+  <si>
+    <t>I - include pronoun (and maybe an extra word?)</t>
+  </si>
+  <si>
+    <t>Minun olisi hyvä</t>
+  </si>
+  <si>
+    <t>### kävellä joka päivä</t>
+  </si>
+  <si>
+    <t>It would be a good idea for me to walk every day</t>
+  </si>
+  <si>
+    <t>U2-13</t>
+  </si>
+  <si>
+    <t>You (singular) - include pronoun (and maybe another word?)</t>
+  </si>
+  <si>
+    <t>Sinun ei ole pakko</t>
+  </si>
+  <si>
+    <t>### laulaa</t>
+  </si>
+  <si>
+    <t>You (singular) must not sing</t>
+  </si>
+  <si>
+    <t>U2-14</t>
+  </si>
+  <si>
+    <t>Matti - include pronoun (and maybe another word?)</t>
+  </si>
+  <si>
+    <t>Mattin ei ole pakko</t>
+  </si>
+  <si>
+    <t>### juosta koska hänellä on polvi kipeä</t>
+  </si>
+  <si>
+    <t>Matti must not run because he has a hurt knee</t>
+  </si>
+  <si>
+    <t>U2-15</t>
+  </si>
+  <si>
+    <t>Pekka - include pronoun</t>
+  </si>
+  <si>
+    <t>Pekkan ei ole pakko</t>
+  </si>
+  <si>
+    <t>### ajaa autoa koska hän on pyöräilijäksi</t>
+  </si>
+  <si>
+    <t>Pekka must not drive because he is the cyclist of the year</t>
+  </si>
+  <si>
+    <t>U2-16</t>
+  </si>
+  <si>
+    <t>She - inclue pronoun (and maybe an extra word?)</t>
+  </si>
+  <si>
+    <t>Hänen olisi hyvä</t>
+  </si>
+  <si>
+    <t>### juoda teeta koska hänellä on kylmä</t>
+  </si>
+  <si>
+    <t>It would be a good idea for her to drink tea, becuase she is cold.</t>
+  </si>
+  <si>
+    <t>U2-17</t>
+  </si>
+  <si>
+    <t>Oppetaja - include pronoun</t>
+  </si>
+  <si>
+    <t>Oppetajan täytyy</t>
+  </si>
+  <si>
+    <t>### nukua</t>
+  </si>
+  <si>
+    <t>The student needs to sleep</t>
+  </si>
+  <si>
+    <t>U2-18</t>
+  </si>
+  <si>
+    <t>Lucca and Kira - include pronoun</t>
+  </si>
+  <si>
+    <t>Luccan ja Kiran täytyy</t>
+  </si>
+  <si>
+    <t>### syödä lihaa.</t>
+  </si>
+  <si>
+    <t>Lucca and Kira need to eat meat</t>
+  </si>
+  <si>
+    <t>U2-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They - include pronoun  </t>
+  </si>
+  <si>
+    <t>Heidän pitää</t>
+  </si>
+  <si>
+    <t>### ostaa kissanruoka</t>
+  </si>
+  <si>
+    <t>They need to buy cat food</t>
+  </si>
+  <si>
+    <t>U2-20</t>
+  </si>
+  <si>
+    <t>Bertie - include pronoun</t>
+  </si>
+  <si>
+    <t>Bertien ei pitäisi</t>
+  </si>
+  <si>
+    <t>### puraista Lucca</t>
+  </si>
+  <si>
+    <t>Bertie should not bite Luuca</t>
+  </si>
+  <si>
+    <t>U2-21</t>
+  </si>
+  <si>
+    <t>We - include pronoun</t>
+  </si>
+  <si>
+    <t>Meidän pitäisi</t>
+  </si>
+  <si>
+    <t>### siivota</t>
+  </si>
+  <si>
+    <t>We should clean</t>
+  </si>
+  <si>
+    <t>U2-22</t>
+  </si>
+  <si>
+    <t>Me tarvitsimme</t>
+  </si>
+  <si>
+    <t>We need potatoes!</t>
+  </si>
+  <si>
+    <t>U2-23</t>
+  </si>
+  <si>
+    <t>Meidän ei tarvitse</t>
+  </si>
+  <si>
+    <t>### ajaa autoa suomessa.</t>
+  </si>
+  <si>
+    <t>We do not need to drive in Finland.</t>
+  </si>
+  <si>
+    <t>U2-24</t>
+  </si>
+  <si>
+    <t>Kaikki - include pronoun</t>
+  </si>
+  <si>
+    <t>Kaikkien pitäisi</t>
+  </si>
+  <si>
+    <t>### puhua suomea</t>
+  </si>
+  <si>
+    <t>Everyone should speak Finnish.</t>
+  </si>
+  <si>
+    <t>U2-25</t>
+  </si>
+  <si>
+    <t>Michellen pitää</t>
+  </si>
+  <si>
+    <t>### lisätä maitoa ja sokeria kahviinsa</t>
+  </si>
+  <si>
+    <t>Michelle needs to add milk and sugar to her coffee</t>
+  </si>
+  <si>
+    <t>U2-26</t>
+  </si>
+  <si>
+    <t>She - include pronoun</t>
+  </si>
+  <si>
+    <t>Hänen täytyy</t>
+  </si>
+  <si>
+    <t>### korjata pyoränsä</t>
+  </si>
+  <si>
+    <t>She needs to fix her bike</t>
+  </si>
+  <si>
+    <t>U2-27</t>
+  </si>
+  <si>
+    <t>They - include pronoun</t>
+  </si>
+  <si>
+    <t>Heidän täytyy</t>
+  </si>
+  <si>
+    <t>### lainata kirja kirjastosta</t>
+  </si>
+  <si>
+    <t>They need to borrow a book from the library</t>
+  </si>
+  <si>
+    <t>U2-28</t>
+  </si>
+  <si>
+    <t>They - include pronoune</t>
+  </si>
+  <si>
+    <t>He tarvitsevat</t>
+  </si>
+  <si>
+    <t>### kirja kirjastosta</t>
+  </si>
+  <si>
+    <t>They need a book from the library</t>
+  </si>
+  <si>
+    <t>U2-29</t>
+  </si>
+  <si>
+    <t>Kaikki - include pronoun (and another word?)</t>
+  </si>
+  <si>
+    <t>Kaikkien on pakko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">### olla hiljaa yöllä rakennuksessa </t>
+  </si>
+  <si>
+    <t>Everyone must be quiet at night in the building</t>
+  </si>
+  <si>
+    <t>U2-30</t>
+  </si>
+  <si>
+    <t>Teidän pitää</t>
+  </si>
+  <si>
+    <t>### joskus katsoa ulos</t>
+  </si>
+  <si>
+    <t>You (plural) need to look outside sometime</t>
   </si>
 </sst>
 </file>
@@ -1104,6 +1534,10 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2454,183 +2888,180 @@
       <c r="A1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>270</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>196</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>230</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -2657,7 +3088,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B1" s="1">
         <v>0.0</v>
@@ -2665,250 +3096,250 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>132</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>230</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>158</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -2936,7 +3367,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B1" s="1">
         <v>1.0</v>
@@ -2944,132 +3375,1000 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>132</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="H10" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.86"/>
+    <col customWidth="1" min="2" max="2" width="14.0"/>
+    <col customWidth="1" min="5" max="6" width="24.29"/>
+    <col customWidth="1" min="7" max="7" width="42.0"/>
+    <col customWidth="1" min="8" max="8" width="46.43"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="G10" s="1" t="s">
-        <v>326</v>
+        <v>347</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>327</v>
+        <v>355</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing bug in display of wrong answer text.  Also updating Excel spreadsheet to fix incorrect sentences.
</commit_message>
<xml_diff>
--- a/data/OpinSuomea - Lause tiedot.xlsx
+++ b/data/OpinSuomea - Lause tiedot.xlsx
@@ -1120,7 +1120,7 @@
     <t>U1-5</t>
   </si>
   <si>
-    <t>syömme</t>
+    <t>syötte</t>
   </si>
   <si>
     <t>Te ###.</t>
@@ -1132,7 +1132,7 @@
     <t>U1-6</t>
   </si>
   <si>
-    <t>juovät</t>
+    <t>juovat</t>
   </si>
   <si>
     <t>He ###.</t>
@@ -1576,7 +1576,7 @@
     <t>You (plural) need to look outside sometime</t>
   </si>
   <si>
-    <t>Posposition locaitons</t>
+    <t>Postposition locaitons</t>
   </si>
   <si>
     <t>A range of sentences to test locative post-positions.</t>
@@ -1660,7 +1660,7 @@
     <t>tuolin takana</t>
   </si>
   <si>
-    <t>Sinun kirjä on ###</t>
+    <t>Sinun kirja on ###</t>
   </si>
   <si>
     <t>Your book is behind the chair</t>
@@ -1672,7 +1672,7 @@
     <t>puolin taakse</t>
   </si>
   <si>
-    <t>Sinun kirjä putoaa ###</t>
+    <t>Sinun kirja putoaa ###</t>
   </si>
   <si>
     <t>Your book falls behind the chair</t>
@@ -1807,7 +1807,7 @@
     <t>U3-17</t>
   </si>
   <si>
-    <t>meidän eteen</t>
+    <t>sinun eteen</t>
   </si>
   <si>
     <t>Supersankari hyppää ###</t>
@@ -2056,7 +2056,7 @@
     <t>U3-35</t>
   </si>
   <si>
-    <t>kirjän keskellä</t>
+    <t>kirjan keskellä</t>
   </si>
   <si>
     <t>Kartta on ###</t>
@@ -2333,7 +2333,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2343,10 +2343,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <name val="Arial"/>
-    </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
@@ -2372,29 +2368,26 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -4034,7 +4027,7 @@
       <c r="A3" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>321</v>
       </c>
     </row>
@@ -4042,7 +4035,7 @@
       <c r="A4" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>322</v>
       </c>
     </row>
@@ -4050,7 +4043,7 @@
       <c r="A5" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>323</v>
       </c>
     </row>
@@ -4124,7 +4117,7 @@
       <c r="G9" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="1" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4193,7 +4186,7 @@
       <c r="F12" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="1" t="s">
         <v>341</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -4240,7 +4233,7 @@
       <c r="F14" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="1" t="s">
         <v>345</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -4271,7 +4264,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>347</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -4281,38 +4274,38 @@
         <v>296</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="4" t="s">
         <v>349</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>308</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="6"/>
-      <c r="AB16" s="6"/>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="6"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
     </row>
     <row r="17">
       <c r="B17" s="1" t="s">
@@ -4331,18 +4324,18 @@
       <c r="G17" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="1" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="1" t="s">
         <v>353</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="1" t="s">
         <v>354</v>
       </c>
     </row>
@@ -4381,7 +4374,7 @@
       <c r="A2" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>355</v>
       </c>
     </row>
@@ -4389,7 +4382,7 @@
       <c r="A3" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>356</v>
       </c>
     </row>
@@ -4397,7 +4390,7 @@
       <c r="A4" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>322</v>
       </c>
     </row>
@@ -4405,7 +4398,7 @@
       <c r="A5" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>357</v>
       </c>
     </row>
@@ -4517,7 +4510,7 @@
       <c r="C11" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="1" t="s">
         <v>172</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -4540,16 +4533,16 @@
       <c r="C12" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="1" t="s">
         <v>367</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="1" t="s">
         <v>369</v>
       </c>
     </row>
@@ -4557,7 +4550,7 @@
       <c r="A13" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -4634,7 +4627,7 @@
       <c r="A5" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>377</v>
       </c>
     </row>
@@ -5096,7 +5089,7 @@
       <c r="E24" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="1" t="s">
         <v>456</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -5478,7 +5471,7 @@
       <c r="A2" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>519</v>
       </c>
     </row>
@@ -5486,7 +5479,7 @@
       <c r="A3" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>520</v>
       </c>
     </row>
@@ -5494,7 +5487,7 @@
       <c r="A4" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>322</v>
       </c>
     </row>
@@ -5502,7 +5495,7 @@
       <c r="A5" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>521</v>
       </c>
     </row>
@@ -5755,7 +5748,7 @@
       <c r="F17" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="1" t="s">
         <v>565</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -5907,7 +5900,7 @@
       <c r="C24" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>596</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -6617,7 +6610,7 @@
       <c r="C56" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="1" t="s">
         <v>740</v>
       </c>
       <c r="G56" s="1" t="s">
@@ -6640,7 +6633,7 @@
       <c r="C57" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="F57" s="1" t="s">
         <v>745</v>
       </c>
       <c r="G57" s="1" t="s">
@@ -6709,7 +6702,7 @@
       <c r="F60" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="G60" s="4" t="s">
+      <c r="G60" s="1" t="s">
         <v>757</v>
       </c>
       <c r="H60" s="1" t="s">
@@ -6732,7 +6725,7 @@
       <c r="F61" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="G61" s="4" t="s">
+      <c r="G61" s="1" t="s">
         <v>757</v>
       </c>
       <c r="H61" s="1" t="s">
@@ -6752,7 +6745,7 @@
       <c r="F62" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="G62" s="1" t="s">
         <v>765</v>
       </c>
       <c r="H62" s="1" t="s">

</xml_diff>

<commit_message>
Fixing menu display issues. Updating readme
</commit_message>
<xml_diff>
--- a/data/OpinSuomea - Lause tiedot.xlsx
+++ b/data/OpinSuomea - Lause tiedot.xlsx
@@ -1669,7 +1669,7 @@
     <t>U3-7</t>
   </si>
   <si>
-    <t>puolin taakse</t>
+    <t>tuolin taakse</t>
   </si>
   <si>
     <t>Sinun kirja putoaa ###</t>
@@ -1711,7 +1711,7 @@
     <t>Lumi</t>
   </si>
   <si>
-    <t>Lumen alla</t>
+    <t>lumen alla</t>
   </si>
   <si>
     <t>Penkki on ###</t>
@@ -1726,7 +1726,7 @@
     <t>Huopa (watch consonant gradation!)</t>
   </si>
   <si>
-    <t>Huoppan alla</t>
+    <t>huoppan alla</t>
   </si>
   <si>
     <t>Michelle on ###</t>
@@ -1738,7 +1738,7 @@
     <t>U3-12</t>
   </si>
   <si>
-    <t>Puun alle</t>
+    <t>puun alle</t>
   </si>
   <si>
     <t>He juoksevat ###</t>
@@ -1768,7 +1768,7 @@
     <t>Kaupa</t>
   </si>
   <si>
-    <t>Kaupan edessä</t>
+    <t>kaupan edessä</t>
   </si>
   <si>
     <t>Odotan ###</t>
@@ -2080,7 +2080,7 @@
     <t>U3-37</t>
   </si>
   <si>
-    <t>pullan keskelta</t>
+    <t>pullan keskeltä</t>
   </si>
   <si>
     <t>Hillo putoaa ###</t>
@@ -2113,7 +2113,7 @@
     <t>lattia</t>
   </si>
   <si>
-    <t>lattia keskelle</t>
+    <t>lattian keskelle</t>
   </si>
   <si>
     <t>Laitamme maton ###</t>
@@ -2167,7 +2167,7 @@
     <t>kirkko</t>
   </si>
   <si>
-    <t>kirkon viressä</t>
+    <t>kirkon vieressä</t>
   </si>
   <si>
     <t>The store is next to the church</t>

</xml_diff>